<commit_message>
check if pushing works properly
</commit_message>
<xml_diff>
--- a/datasheet.xlsx
+++ b/datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanblackmore/Documents/AA Studie/Master/Q1/Operations Optimisation/MILP_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1A9ED7-415B-F440-B749-45DDB8E08232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA08C7A4-70F7-0041-92D6-BAE80DA1354B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-920" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{5F5361A1-35E0-444D-99D6-775B076FC792}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" activeTab="3" xr2:uid="{5F5361A1-35E0-444D-99D6-775B076FC792}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA77DD9-315F-D64B-9217-F60AC5E2FC2E}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1106,9 +1106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E3C333-77AE-4145-BF56-652F0C24E420}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1852,8 +1850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E4D0F8-9C33-8041-8AC2-67D48777EAA4}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="164" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1877,13 +1875,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>